<commit_message>
Changes to Acadis Summary
</commit_message>
<xml_diff>
--- a/Acadis Complete Crawl Histogram and summary.xlsx
+++ b/Acadis Complete Crawl Histogram and summary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>application/zip</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Extension</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
@@ -571,18 +577,18 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1658,26 +1664,26 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="72639232"/>
-        <c:axId val="72640768"/>
+        <c:axId val="81673600"/>
+        <c:axId val="81687680"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="72639232"/>
+        <c:axId val="81673600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72640768"/>
+        <c:crossAx val="81687680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72640768"/>
+        <c:axId val="81687680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1685,7 +1691,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72639232"/>
+        <c:crossAx val="81673600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1697,7 +1703,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.67030970120194178"/>
-          <c:y val="8.0057974191741113E-2"/>
+          <c:y val="8.0057974191741141E-2"/>
           <c:w val="0.31876133861690709"/>
           <c:h val="0.82750948474828112"/>
         </c:manualLayout>
@@ -1707,7 +1713,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2035,52 +2041,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D15" sqref="C15:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B2">
@@ -2118,7 +2124,7 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B3">
@@ -2156,7 +2162,7 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B4">
@@ -2194,7 +2200,7 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B5">
@@ -2232,7 +2238,7 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B6">
@@ -2270,7 +2276,7 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7">
@@ -2308,7 +2314,7 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8">
@@ -2346,7 +2352,7 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9">
@@ -2384,7 +2390,7 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B10">
@@ -2422,7 +2428,7 @@
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B11">
@@ -2460,234 +2466,238 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="3">
         <v>1</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="4">
         <v>2.101723413198823E-5</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="6">
         <v>8014</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <v>0.16843211433375369</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="3"/>
-      <c r="B18" s="8" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="6">
         <v>6</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="5">
         <v>1.2610340479192938E-4</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="3">
         <v>1</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="4">
         <v>2.101723413198823E-5</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="3">
         <v>7</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="4">
         <v>1.4712063892391761E-4</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="1"/>
-      <c r="B21" s="5" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="3">
         <v>1</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="4">
         <v>2.101723413198823E-5</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="1"/>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="3">
         <v>12</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="4">
         <v>2.5220680958385876E-4</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="3">
         <v>1</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="4">
         <v>2.101723413198823E-5</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="1"/>
-      <c r="B24" s="5" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="3">
         <v>2350</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="4">
         <v>4.9390500210172342E-2</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="1"/>
-      <c r="B25" s="5" t="s">
+      <c r="A25" s="8"/>
+      <c r="B25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="3">
         <v>20351</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="4">
         <v>0.42772173182009249</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="1"/>
-      <c r="B26" s="5" t="s">
+      <c r="A26" s="8"/>
+      <c r="B26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="3">
         <v>6</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="4">
         <v>1.2610340479192938E-4</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="6">
         <v>8102</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="5">
         <v>0.17028163093736864</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="3">
         <v>1</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="4">
         <v>2.101723413198823E-5</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="3">
         <v>8100</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="4">
         <v>0.17023959646910466</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="3">
         <v>626</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="4">
         <v>1.3156788566624632E-2</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="3">
         <v>1</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="4">
         <v>2.101723413198823E-5</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3">
         <v>47580</v>
       </c>
-      <c r="D32" s="5"/>
+      <c r="D32" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2696,7 +2706,8 @@
     <mergeCell ref="A23:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>